<commit_message>
heater numbers changed to 20 and burner numbers changed to 3
</commit_message>
<xml_diff>
--- a/temp/combustion calculation.xlsx
+++ b/temp/combustion calculation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSST\معاینه فنی موتورخانه\calculation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hossein.sharifi\PycharmProjects\pyqtdesigner\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="محاسبات راندمان" sheetId="2" r:id="rId1"/>
@@ -667,6 +667,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -699,13 +705,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -962,8 +962,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="129069656"/>
-        <c:axId val="129069264"/>
+        <c:axId val="175259280"/>
+        <c:axId val="175259840"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1065,11 +1065,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="129067696"/>
-        <c:axId val="129068872"/>
+        <c:axId val="175260960"/>
+        <c:axId val="175260400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="129069656"/>
+        <c:axId val="175259280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -1127,13 +1127,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129069264"/>
+        <c:crossAx val="175259840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="129069264"/>
+        <c:axId val="175259840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,13 +1190,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129069656"/>
+        <c:crossAx val="175259280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="129068872"/>
+        <c:axId val="175260400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,12 +1239,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129067696"/>
+        <c:crossAx val="175260960"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="129067696"/>
+        <c:axId val="175260960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129068872"/>
+        <c:crossAx val="175260400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2159,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:K14"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2217,70 +2217,76 @@
         <v>45</v>
       </c>
       <c r="B2" s="2">
-        <v>91.167143987812693</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>3.076174585996085</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>0.80312332592328162</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>0.37731073648288038</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2">
-        <v>0.15889400436066498</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2">
-        <v>0.80747498753273916</v>
+        <v>0</v>
       </c>
       <c r="J2" s="2">
         <v>0</v>
       </c>
       <c r="K2" s="2">
-        <v>3.6098783718916647</v>
-      </c>
-      <c r="L2" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
       <c r="M2" s="2"/>
       <c r="N2" s="1">
-        <f>SUM(B2:K2)</f>
-        <v>100.00000000000001</v>
+        <f>SUM(B2:L2)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="22.5">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="24">
         <f>B19</f>
-        <v>10.202676453896851</v>
+        <v>8.3836351441985251</v>
       </c>
       <c r="J3" s="24"/>
       <c r="K3" s="24">
         <f>100-(I3+L3+M3)</f>
-        <v>87.068027453789412</v>
+        <v>86.082104560037621</v>
       </c>
       <c r="L3" s="24">
         <f>21-(21/B17)</f>
-        <v>2.7292960923137386</v>
+        <v>5.5342602957638594</v>
       </c>
       <c r="M3" s="24">
         <v>0</v>
       </c>
       <c r="N3" s="1"/>
+      <c r="Q3">
+        <f>I3*I5+K3*K5+L3*L5</f>
+        <v>132.11996818459809</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="22.5">
       <c r="A4" s="1" t="s">
@@ -2288,7 +2294,7 @@
       </c>
       <c r="B4" s="1">
         <f>B2/100</f>
-        <v>0.91167143987812693</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <f>C2/100</f>
@@ -2296,7 +2302,7 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" ref="D4:K4" si="0">D2/100</f>
-        <v>3.0761745859960849E-2</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
@@ -2304,19 +2310,19 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>8.0312332592328162E-3</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>3.7731073648288038E-3</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>1.5889400436066498E-3</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>8.0747498753273913E-3</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="0"/>
@@ -2324,7 +2330,7 @@
       </c>
       <c r="K4" s="1">
         <f t="shared" si="0"/>
-        <v>3.6098783718916644E-2</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2332,6 +2338,10 @@
       <c r="O4" s="30" t="s">
         <v>59</v>
       </c>
+      <c r="Q4">
+        <f>Q3/N9</f>
+        <v>8.2354681342781877</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="22.5">
       <c r="A5" s="1" t="s">
@@ -2363,7 +2373,7 @@
       </c>
       <c r="J5" s="25">
         <f>I47</f>
-        <v>0.50403225806451613</v>
+        <v>0.42390843577787196</v>
       </c>
       <c r="K5" s="1">
         <v>1.2504</v>
@@ -2374,11 +2384,11 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1">
         <f>B5*B4+C4*C5+D5*D4+E4*E5+F5*F4+G5*G4+H4*H5+I5*I4+K5*K4</f>
-        <v>0.78797613588788662</v>
+        <v>0.71750000000000003</v>
       </c>
       <c r="O5" s="30">
         <f>(I3*I5+K3*K5+L3*L5)/100</f>
-        <v>1.3294071699348871</v>
+        <v>1.321199681845981</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="22.5">
@@ -2387,7 +2397,7 @@
       </c>
       <c r="B6" s="1">
         <f>B9/$N$9</f>
-        <v>0.83075162179401707</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ref="C6:M6" si="1">C9/$N$9</f>
@@ -2395,7 +2405,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>5.2539625954851052E-2</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -2403,19 +2413,19 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>2.0115743261933175E-2</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>1.2456609905775165E-2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>6.5117320886643563E-3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>2.0185111467801903E-2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
@@ -2423,7 +2433,7 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="1"/>
-        <v>5.7439555526957085E-2</v>
+        <v>0</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="1"/>
@@ -2435,14 +2445,14 @@
       </c>
       <c r="N6" s="1">
         <f>SUM(B6:K6)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="P6" t="s">
         <v>66</v>
       </c>
       <c r="Q6">
         <f>B4*1+D4*2+F4*3+G4*4+H4*5</f>
-        <v>1.0203257610530956</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="22.5">
@@ -2451,7 +2461,7 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ref="B7:L7" si="2">B9/B5</f>
-        <v>20.384338084566988</v>
+        <v>22.359303135888499</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="2"/>
@@ -2459,7 +2469,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>0.68264514006414811</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="2"/>
@@ -2467,19 +2477,19 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" si="2"/>
-        <v>0.17610485730769873</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="2"/>
-        <v>8.097489914926137E-2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="2"/>
-        <v>3.8769707185059114E-2</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>0.17975120235871694</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="2"/>
@@ -2487,7 +2497,7 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>0.80874093716530671</v>
+        <v>0</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="2"/>
@@ -2496,18 +2506,18 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1">
         <f>SUM(B7:K7)</f>
-        <v>22.351324827797178</v>
+        <v>22.359303135888499</v>
       </c>
       <c r="O7">
         <f>N9/N7</f>
-        <v>0.78766954006329759</v>
+        <v>0.71750000000000003</v>
       </c>
       <c r="P7" t="s">
         <v>67</v>
       </c>
       <c r="Q7">
         <f>B4*4+D4*6+F4*8+G4*10+H4*12</f>
-        <v>3.9523044549177033</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="22.5">
@@ -2516,7 +2526,7 @@
       </c>
       <c r="B8" s="1">
         <f>B7/$N$7</f>
-        <v>0.91199686110847655</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ref="C8:M8" si="3">C7/$N$7</f>
@@ -2524,7 +2534,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="3"/>
-        <v>3.0541596318048134E-2</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="3"/>
@@ -2532,19 +2542,19 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" si="3"/>
-        <v>7.8789449244944208E-3</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="3"/>
-        <v>3.6228232452940375E-3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="3"/>
-        <v>1.7345596953986034E-3</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="3"/>
-        <v>8.0420826838492245E-3</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
@@ -2552,7 +2562,7 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="3"/>
-        <v>3.6183132024439006E-2</v>
+        <v>0</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
@@ -2570,7 +2580,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ref="B9:M9" si="4">B4*B13</f>
-        <v>14.625762575676815</v>
+        <v>16.0428</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="4"/>
@@ -2578,7 +2588,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="4"/>
-        <v>0.92498416478692069</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="4"/>
@@ -2586,19 +2596,19 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" si="4"/>
-        <v>0.35414686804578216</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="4"/>
-        <v>0.21930431936594455</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="4"/>
-        <v>0.1146420241462198</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="4"/>
-        <v>0.35536812706318344</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="4"/>
@@ -2606,7 +2616,7 @@
       </c>
       <c r="K9" s="1">
         <f t="shared" si="4"/>
-        <v>1.0112496678314995</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="4"/>
@@ -2618,7 +2628,7 @@
       </c>
       <c r="N9" s="1">
         <f>SUM(B9:M9)</f>
-        <v>17.605457746916368</v>
+        <v>16.0428</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="22.5">
@@ -2657,15 +2667,15 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1">
         <f>(B6*B10+C6*C10+D6*D10+E6*E10+F6*F10+G6*G10+H6*H10)</f>
-        <v>50778.395538937861</v>
+        <v>55499</v>
       </c>
       <c r="O10">
         <f>N10*O7</f>
-        <v>39996.595459307384</v>
+        <v>39820.532500000001</v>
       </c>
       <c r="P10">
         <f>O10-2.036*4.18*480</f>
-        <v>35911.565059307381</v>
+        <v>35735.502099999998</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="22.5">
@@ -2673,27 +2683,27 @@
         <v>23</v>
       </c>
       <c r="B11" s="2">
-        <v>20</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="41"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="43"/>
       <c r="O11">
         <f>N10-B15*2442.5</f>
-        <v>45805.610444454891</v>
+        <v>50011.946617797395</v>
       </c>
       <c r="P11">
         <f>P10/3600</f>
-        <v>9.9754347386964941</v>
+        <v>9.9265283611111101</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="22.5">
@@ -2701,20 +2711,20 @@
         <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>180</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="41"/>
+        <v>250</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="43"/>
     </row>
     <row r="13" spans="1:17" ht="22.5">
       <c r="A13" s="1" t="s">
@@ -2754,32 +2764,32 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1">
         <f>B4*B13+D4*D13+F4*F13+G4*G13+I4*I13+K4*K13</f>
-        <v>17.490815722770147</v>
+        <v>16.0428</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="22.5">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="43"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="1">
         <f>2*B4*J13+2*C4*J13+3*D4*J13+3*E4*J13+4*F4*J13+5*G4*J13+6*H4*J13</f>
-        <v>35.610263138808513</v>
+        <v>36.04</v>
       </c>
       <c r="O14">
         <f>0.07016+0.04084*(N10/1000)</f>
-        <v>2.1439496738102224</v>
+        <v>2.33673916</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="22.5">
@@ -2788,23 +2798,23 @@
       </c>
       <c r="B15" s="1">
         <f>N14/N13</f>
-        <v>2.0359406732785965</v>
-      </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="41"/>
+        <v>2.2464906375445683</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="43"/>
       <c r="O15">
         <f>0.07793+0.04537*(O11/1000)</f>
-        <v>2.1561305458649183</v>
+        <v>2.3469720180494678</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="22.5">
@@ -2812,7 +2822,7 @@
         <v>58</v>
       </c>
       <c r="B16" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
@@ -2833,42 +2843,42 @@
       </c>
       <c r="B17" s="1">
         <f>1+((N17/G17)*(B16/(21-B16)))</f>
-        <v>1.1493810039341481</v>
+        <v>1.3578399999999999</v>
       </c>
       <c r="C17" s="1">
         <f>B17-1</f>
-        <v>0.1493810039341481</v>
-      </c>
-      <c r="D17" s="44" t="s">
+        <v>0.35783999999999994</v>
+      </c>
+      <c r="D17" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="8">
         <f>1/0.21*(2*B4+3*C4+3.5*D4+4.5*E4+5*F4+6.5*G4+8*H4)</f>
-        <v>9.5638184513453393</v>
-      </c>
-      <c r="H17" s="44" t="s">
+        <v>9.5238095238095237</v>
+      </c>
+      <c r="H17" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="46"/>
+      <c r="I17" s="33"/>
       <c r="J17" s="8">
         <f>L17+N17</f>
-        <v>10.548069037694226</v>
+        <v>10.52</v>
       </c>
       <c r="K17" s="29" t="s">
         <v>54</v>
       </c>
       <c r="L17" s="8">
         <f>2*B4+2*C4+3*D4+3*E4+4*F4+5*G4+6*H4</f>
-        <v>1.9761522274588517</v>
+        <v>2</v>
       </c>
       <c r="M17" s="29" t="s">
         <v>55</v>
       </c>
       <c r="N17" s="8">
         <f>1*B4+2*C4+2*D4+3*E4+3*F4+4*G4+5*H4+3.76*(2*B4+3*C4+3.5*D4+4.5*E4+5*F4+6.5*G4+8*H4)</f>
-        <v>8.5719168102353738</v>
+        <v>8.52</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="22.5">
@@ -2877,7 +2887,7 @@
       </c>
       <c r="B18" s="24">
         <f>100/N17*(B4+2*C4+2*D4+3*E4+3*F4+4*G4+5*H4)</f>
-        <v>11.903122529546327</v>
+        <v>11.737089201877934</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
@@ -2898,7 +2908,7 @@
       </c>
       <c r="B19" s="24">
         <f>B18*((21-B16)/21)</f>
-        <v>10.202676453896851</v>
+        <v>8.3836351441985251</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -2912,6 +2922,10 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
+      <c r="O19">
+        <f>(N17*B17*O5)/N5</f>
+        <v>21.30270474076767</v>
+      </c>
     </row>
     <row r="20" spans="1:18" ht="22.5">
       <c r="A20" s="1" t="s">
@@ -2919,20 +2933,20 @@
       </c>
       <c r="B20" s="1">
         <f>B6*(I13+C17*2*32+((1+C17)*0.79/0.21*2*K13))+C6*(2*I13+C17*3*32+((1+C17)*0.79/0.21*3*K13))+D6*(2*I13+C17*3.5*32+((1+C17)*0.79/0.21*3.5*K13))+E6*(3*I13+C17*4.5*32+((1+C17)*0.79/0.21*4.5*K13))+F6*(3*I13+C17*5*32+((1+C17)*0.79/0.21*5*K13))+G6*(4*I13+C17*6.5*32+((1+C17)*0.79/0.21*6.5*K13))+H6*(5*I13+C17*8*32+((1+C17)*0.79/0.21*8*K13))+I6*I13+K6*K13</f>
-        <v>311.72798270457116</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="41"/>
+        <v>353.10008280228573</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="43"/>
     </row>
     <row r="21" spans="1:18" ht="22.5">
       <c r="A21" s="1" t="s">
@@ -2940,20 +2954,20 @@
       </c>
       <c r="B21" s="1">
         <f>B20/N13</f>
-        <v>17.822381051030852</v>
-      </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="41"/>
+        <v>22.009878749487978</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="43"/>
     </row>
     <row r="22" spans="1:18" ht="22.5">
       <c r="A22" s="1" t="s">
@@ -2961,7 +2975,7 @@
       </c>
       <c r="B22" s="1">
         <f ca="1">(E49+E56)/(2*O5)</f>
-        <v>1.0080338986113764</v>
+        <v>1.0137940781789812</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
@@ -2982,7 +2996,7 @@
       </c>
       <c r="B23" s="1">
         <f>(D48+D55)/(2*J5)</f>
-        <v>2.8440639999999999</v>
+        <v>3.4016780000000004</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
@@ -3003,20 +3017,20 @@
       </c>
       <c r="B24" s="1">
         <f ca="1">B21*B22*(B12-B11)+B15*B23*(B12-B11)</f>
-        <v>3800.9455725464909</v>
-      </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="41"/>
+        <v>7488.8306291524113</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="43"/>
     </row>
     <row r="25" spans="1:18" ht="22.5">
       <c r="A25" s="3" t="s">
@@ -3024,30 +3038,30 @@
       </c>
       <c r="B25" s="3">
         <f ca="1">(1-(B24/N10))*100</f>
-        <v>92.51464026737149</v>
-      </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="41"/>
+        <v>86.506368350506463</v>
+      </c>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="43"/>
     </row>
     <row r="29" spans="1:18" ht="15.75">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43" t="s">
+      <c r="B29" s="44"/>
+      <c r="C29" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="43"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="K29" s="10"/>
@@ -3056,17 +3070,17 @@
       <c r="N29" s="10"/>
     </row>
     <row r="30" spans="1:18" ht="18">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34" t="s">
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
@@ -3494,11 +3508,11 @@
       <c r="C44" s="27"/>
       <c r="D44" s="27"/>
       <c r="E44" s="28"/>
-      <c r="I44" s="32" t="s">
+      <c r="I44" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="9" t="s">
@@ -3506,7 +3520,7 @@
       </c>
       <c r="B45" s="15">
         <f>B12</f>
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="C45" s="16">
         <v>0</v>
@@ -3518,7 +3532,7 @@
       </c>
       <c r="J45" s="15">
         <f>B12</f>
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="K45" s="16">
         <v>0</v>
@@ -3547,15 +3561,15 @@
     <row r="47" spans="1:18">
       <c r="A47" s="15">
         <f>I3</f>
-        <v>10.202676453896851</v>
+        <v>8.3836351441985251</v>
       </c>
       <c r="B47" s="15">
         <f>L3</f>
-        <v>2.7292960923137386</v>
+        <v>5.5342602957638594</v>
       </c>
       <c r="C47" s="18">
         <f>K3</f>
-        <v>87.068027453789412</v>
+        <v>86.082104560037621</v>
       </c>
       <c r="D47" s="18"/>
       <c r="E47" s="18">
@@ -3564,45 +3578,45 @@
       </c>
       <c r="I47" s="19">
         <f>(LOOKUP(J45+100,I32:I42,K32:K42)-LOOKUP(J45,I32:I42,K32:K42))/100*K45+LOOKUP(J45,I32:I42,K32:K42)</f>
-        <v>0.50403225806451613</v>
+        <v>0.42390843577787196</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="19">
         <f>(LOOKUP(B45+100,A32:A42,B32:B42)-LOOKUP(B45,A32:A42,B32:B42))/100*C45+LOOKUP(B45,A32:A42,B32:B42)</f>
-        <v>1.7250000000000001</v>
+        <v>1.8080000000000001</v>
       </c>
       <c r="B48" s="19">
         <f ca="1">(LOOKUP(B45+100,A32:A42,C32:C37)-LOOKUP(B45,A32:A42,C32:C42))/100*C45+LOOKUP(B45,A32:A42,C32:C42)</f>
-        <v>1.319</v>
+        <v>1.34</v>
       </c>
       <c r="C48" s="19">
         <f>(LOOKUP(B45+100,A32:A42,D32:D42)-LOOKUP(B45,A32:A42,D32:D42))/100*C45+LOOKUP(B45,A32:A42,D32:D42)</f>
-        <v>1.302</v>
+        <v>1.306</v>
       </c>
       <c r="D48" s="19">
         <f>(LOOKUP(B45+100,A32:A42,E32:E42)-LOOKUP(B45,A32:A42,E32:E42))/100*C45+LOOKUP(B45,A32:A42,E32:E42)</f>
-        <v>1.44</v>
+        <v>1.4570000000000001</v>
       </c>
       <c r="E48" s="20"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="21">
         <f>A48*A47/100</f>
-        <v>0.17599616882972069</v>
+        <v>0.15157612340710933</v>
       </c>
       <c r="B49" s="21">
         <f ca="1">B48*B47/100</f>
-        <v>3.5999415457618207E-2</v>
+        <v>7.4159087963235726E-2</v>
       </c>
       <c r="C49" s="21">
         <f>C48*C47/100</f>
-        <v>1.1336257174483382</v>
+        <v>1.1242322855540914</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="22">
         <f ca="1">SUM(A49:C49)</f>
-        <v>1.3456213017356771</v>
+        <v>1.3499674969244364</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3614,12 +3628,12 @@
     </row>
     <row r="51" spans="1:5" ht="19.5">
       <c r="A51" s="14"/>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
@@ -3627,7 +3641,7 @@
       </c>
       <c r="B52" s="15">
         <f>B11</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C52" s="16">
         <v>0</v>
@@ -3655,15 +3669,15 @@
     <row r="54" spans="1:5">
       <c r="A54" s="15">
         <f>A47</f>
-        <v>10.202676453896851</v>
+        <v>8.3836351441985251</v>
       </c>
       <c r="B54" s="15">
         <f>B47</f>
-        <v>2.7292960923137386</v>
+        <v>5.5342602957638594</v>
       </c>
       <c r="C54" s="18">
         <f>C47</f>
-        <v>87.068027453789412</v>
+        <v>86.082104560037621</v>
       </c>
       <c r="D54" s="18"/>
       <c r="E54" s="18">
@@ -3693,41 +3707,41 @@
     <row r="56" spans="1:5">
       <c r="A56" s="21">
         <f>A55*A54/100</f>
-        <v>0.16528335855312901</v>
+        <v>0.13581488933601613</v>
       </c>
       <c r="B56" s="21">
         <f>B55*B54/100</f>
-        <v>3.5644606965617429E-2</v>
+        <v>7.2277439462676007E-2</v>
       </c>
       <c r="C56" s="21">
         <f>C55*C54/100</f>
-        <v>1.1336257174483382</v>
+        <v>1.1207890013716899</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="22">
         <f>SUM(A56:C56)</f>
-        <v>1.3345536829670845</v>
+        <v>1.3288813301703821</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="C20:N20"/>
+    <mergeCell ref="C21:N21"/>
+    <mergeCell ref="C24:N24"/>
+    <mergeCell ref="C25:N25"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="D17:F17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="I44:K44"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="C20:N20"/>
-    <mergeCell ref="C21:N21"/>
-    <mergeCell ref="C24:N24"/>
-    <mergeCell ref="C25:N25"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
some minor changes for creating exe 32bit file with pyinstaller
</commit_message>
<xml_diff>
--- a/temp/combustion calculation.xlsx
+++ b/temp/combustion calculation.xlsx
@@ -667,22 +667,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -701,12 +685,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -962,8 +962,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="175259280"/>
-        <c:axId val="175259840"/>
+        <c:axId val="155040336"/>
+        <c:axId val="155040896"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1065,11 +1065,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="175260960"/>
-        <c:axId val="175260400"/>
+        <c:axId val="155042016"/>
+        <c:axId val="155041456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="175259280"/>
+        <c:axId val="155040336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -1127,13 +1127,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175259840"/>
+        <c:crossAx val="155040896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="175259840"/>
+        <c:axId val="155040896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,13 +1190,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175259280"/>
+        <c:crossAx val="155040336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="175260400"/>
+        <c:axId val="155041456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,12 +1239,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175260960"/>
+        <c:crossAx val="155042016"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="175260960"/>
+        <c:axId val="155042016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175260400"/>
+        <c:crossAx val="155041456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2160,7 +2160,7 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2259,25 +2259,25 @@
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="24">
         <f>B19</f>
-        <v>8.3836351441985251</v>
+        <v>7.8247261345852888</v>
       </c>
       <c r="J3" s="24"/>
       <c r="K3" s="24">
         <f>100-(I3+L3+M3)</f>
-        <v>86.082104560037621</v>
+        <v>85.685050691228298</v>
       </c>
       <c r="L3" s="24">
         <f>21-(21/B17)</f>
-        <v>5.5342602957638594</v>
+        <v>6.4902231741864167</v>
       </c>
       <c r="M3" s="24">
         <v>0</v>
@@ -2285,7 +2285,7 @@
       <c r="N3" s="1"/>
       <c r="Q3">
         <f>I3*I5+K3*K5+L3*L5</f>
-        <v>132.11996818459809</v>
+        <v>131.88459986829938</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="22.5">
@@ -2340,7 +2340,7 @@
       </c>
       <c r="Q4">
         <f>Q3/N9</f>
-        <v>8.2354681342781877</v>
+        <v>8.2207968601677628</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="22.5">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="O5" s="30">
         <f>(I3*I5+K3*K5+L3*L5)/100</f>
-        <v>1.321199681845981</v>
+        <v>1.3188459986829937</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="22.5">
@@ -2683,20 +2683,20 @@
         <v>23</v>
       </c>
       <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="43"/>
+        <v>30</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="37"/>
       <c r="O11">
         <f>N10-B15*2442.5</f>
         <v>50011.946617797395</v>
@@ -2713,18 +2713,18 @@
       <c r="B12" s="2">
         <v>250</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="43"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="37"/>
     </row>
     <row r="13" spans="1:17" ht="22.5">
       <c r="A13" s="1" t="s">
@@ -2771,16 +2771,16 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="43"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="1">
@@ -2800,18 +2800,18 @@
         <f>N14/N13</f>
         <v>2.2464906375445683</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="43"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="37"/>
       <c r="O15">
         <f>0.07793+0.04537*(O11/1000)</f>
         <v>2.3469720180494678</v>
@@ -2822,7 +2822,7 @@
         <v>58</v>
       </c>
       <c r="B16" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
@@ -2843,25 +2843,25 @@
       </c>
       <c r="B17" s="1">
         <f>1+((N17/G17)*(B16/(21-B16)))</f>
-        <v>1.3578399999999999</v>
+        <v>1.4473</v>
       </c>
       <c r="C17" s="1">
         <f>B17-1</f>
-        <v>0.35783999999999994</v>
-      </c>
-      <c r="D17" s="32" t="s">
+        <v>0.44730000000000003</v>
+      </c>
+      <c r="D17" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="33"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="8">
         <f>1/0.21*(2*B4+3*C4+3.5*D4+4.5*E4+5*F4+6.5*G4+8*H4)</f>
         <v>9.5238095238095237</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="33"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="8">
         <f>L17+N17</f>
         <v>10.52</v>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B19" s="24">
         <f>B18*((21-B16)/21)</f>
-        <v>8.3836351441985251</v>
+        <v>7.8247261345852888</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
@@ -2924,7 +2924,7 @@
       <c r="N19" s="8"/>
       <c r="O19">
         <f>(N17*B17*O5)/N5</f>
-        <v>21.30270474076767</v>
+        <v>22.66576269599442</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="22.5">
@@ -2933,20 +2933,20 @@
       </c>
       <c r="B20" s="1">
         <f>B6*(I13+C17*2*32+((1+C17)*0.79/0.21*2*K13))+C6*(2*I13+C17*3*32+((1+C17)*0.79/0.21*3*K13))+D6*(2*I13+C17*3.5*32+((1+C17)*0.79/0.21*3.5*K13))+E6*(3*I13+C17*4.5*32+((1+C17)*0.79/0.21*4.5*K13))+F6*(3*I13+C17*5*32+((1+C17)*0.79/0.21*5*K13))+G6*(4*I13+C17*6.5*32+((1+C17)*0.79/0.21*6.5*K13))+H6*(5*I13+C17*8*32+((1+C17)*0.79/0.21*8*K13))+I6*I13+K6*K13</f>
-        <v>353.10008280228573</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="43"/>
+        <v>377.68078207428573</v>
+      </c>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="37"/>
     </row>
     <row r="21" spans="1:18" ht="22.5">
       <c r="A21" s="1" t="s">
@@ -2954,20 +2954,20 @@
       </c>
       <c r="B21" s="1">
         <f>B20/N13</f>
-        <v>22.009878749487978</v>
-      </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="43"/>
+        <v>23.542073832141877</v>
+      </c>
+      <c r="C21" s="35"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="37"/>
     </row>
     <row r="22" spans="1:18" ht="22.5">
       <c r="A22" s="1" t="s">
@@ -2975,7 +2975,7 @@
       </c>
       <c r="B22" s="1">
         <f ca="1">(E49+E56)/(2*O5)</f>
-        <v>1.0137940781789812</v>
+        <v>1.0140035461989834</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
@@ -3017,20 +3017,20 @@
       </c>
       <c r="B24" s="1">
         <f ca="1">B21*B22*(B12-B11)+B15*B23*(B12-B11)</f>
-        <v>7488.8306291524113</v>
-      </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="43"/>
+        <v>6932.988508514527</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="37"/>
     </row>
     <row r="25" spans="1:18" ht="22.5">
       <c r="A25" s="3" t="s">
@@ -3038,30 +3038,30 @@
       </c>
       <c r="B25" s="3">
         <f ca="1">(1-(B24/N10))*100</f>
-        <v>86.506368350506463</v>
-      </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="43"/>
+        <v>87.507903730671671</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="37"/>
     </row>
     <row r="29" spans="1:18" ht="15.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="45" t="s">
+      <c r="B29" s="45"/>
+      <c r="C29" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="45"/>
+      <c r="D29" s="46"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="K29" s="10"/>
@@ -3070,17 +3070,17 @@
       <c r="N29" s="10"/>
     </row>
     <row r="30" spans="1:18" ht="18">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="36" t="s">
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
@@ -3508,11 +3508,11 @@
       <c r="C44" s="27"/>
       <c r="D44" s="27"/>
       <c r="E44" s="28"/>
-      <c r="I44" s="34" t="s">
+      <c r="I44" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="J44" s="34"/>
-      <c r="K44" s="34"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="9" t="s">
@@ -3561,15 +3561,15 @@
     <row r="47" spans="1:18">
       <c r="A47" s="15">
         <f>I3</f>
-        <v>8.3836351441985251</v>
+        <v>7.8247261345852888</v>
       </c>
       <c r="B47" s="15">
         <f>L3</f>
-        <v>5.5342602957638594</v>
+        <v>6.4902231741864167</v>
       </c>
       <c r="C47" s="18">
         <f>K3</f>
-        <v>86.082104560037621</v>
+        <v>85.685050691228298</v>
       </c>
       <c r="D47" s="18"/>
       <c r="E47" s="18">
@@ -3603,20 +3603,20 @@
     <row r="49" spans="1:5">
       <c r="A49" s="21">
         <f>A48*A47/100</f>
-        <v>0.15157612340710933</v>
+        <v>0.14147104851330203</v>
       </c>
       <c r="B49" s="21">
         <f ca="1">B48*B47/100</f>
-        <v>7.4159087963235726E-2</v>
+        <v>8.6968990534097998E-2</v>
       </c>
       <c r="C49" s="21">
         <f>C48*C47/100</f>
-        <v>1.1242322855540914</v>
+        <v>1.1190467620274416</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="22">
         <f ca="1">SUM(A49:C49)</f>
-        <v>1.3499674969244364</v>
+        <v>1.3474868010748415</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3628,12 +3628,12 @@
     </row>
     <row r="51" spans="1:5" ht="19.5">
       <c r="A51" s="14"/>
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="B52" s="15">
         <f>B11</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C52" s="16">
         <v>0</v>
@@ -3669,15 +3669,15 @@
     <row r="54" spans="1:5">
       <c r="A54" s="15">
         <f>A47</f>
-        <v>8.3836351441985251</v>
+        <v>7.8247261345852888</v>
       </c>
       <c r="B54" s="15">
         <f>B47</f>
-        <v>5.5342602957638594</v>
+        <v>6.4902231741864167</v>
       </c>
       <c r="C54" s="18">
         <f>C47</f>
-        <v>86.082104560037621</v>
+        <v>85.685050691228298</v>
       </c>
       <c r="D54" s="18"/>
       <c r="E54" s="18">
@@ -3707,24 +3707,30 @@
     <row r="56" spans="1:5">
       <c r="A56" s="21">
         <f>A55*A54/100</f>
-        <v>0.13581488933601613</v>
+        <v>0.12676056338028169</v>
       </c>
       <c r="B56" s="21">
         <f>B55*B54/100</f>
-        <v>7.2277439462676007E-2</v>
+        <v>8.4762314654874604E-2</v>
       </c>
       <c r="C56" s="21">
         <f>C55*C54/100</f>
-        <v>1.1207890013716899</v>
+        <v>1.1156193599997926</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="22">
         <f>SUM(A56:C56)</f>
-        <v>1.3288813301703821</v>
+        <v>1.3271422380349489</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="C20:N20"/>
     <mergeCell ref="C21:N21"/>
@@ -3736,12 +3742,6 @@
     <mergeCell ref="C15:N15"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>